<commit_message>
Poster design and Groves images with my stuff added
</commit_message>
<xml_diff>
--- a/Cloudy_Data/LineRatios.xlsx
+++ b/Cloudy_Data/LineRatios.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris_000\Documents\GitHub\AGN_SED\Cloudy_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="660" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="660" windowWidth="25365" windowHeight="15300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>temperature</t>
   </si>
@@ -29,11 +34,17 @@
   <si>
     <t>SII Ratio</t>
   </si>
+  <si>
+    <t>OI Ratio</t>
+  </si>
+  <si>
+    <t>NII Ratio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -72,6 +83,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,15 +416,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,57 +434,179 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="1">
+        <f>LOG10(15.7)</f>
+        <v>1.1958996524092338</v>
+      </c>
+      <c r="C2">
+        <f>LOG10(0.159/2.86)</f>
+        <v>-1.2549689088085916</v>
+      </c>
+      <c r="D2">
+        <f>LOG10(0.0355/2.86)</f>
+        <v>-1.9061376800739489</v>
+      </c>
+      <c r="E2">
+        <f>LOG10(1.01/2.86)</f>
+        <v>-0.45204465934640037</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>100000</v>
       </c>
-      <c r="B2">
-        <f>LOG10(15.022)</f>
-        <v>1.176727757644189</v>
-      </c>
-      <c r="C2">
-        <f>LOG10(0.0547)</f>
-        <v>-1.2620126736665693</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>420000</v>
-      </c>
       <c r="B3">
-        <f>LOG10(13.193)</f>
-        <v>1.1203435624380247</v>
+        <f>LOG10(12.9)</f>
+        <v>1.110589710299249</v>
       </c>
       <c r="C3">
-        <f>LOG10(0.0595)</f>
-        <v>-1.2254830342714504</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <f>LOG10(0.131/2.88)</f>
+        <v>-1.3421211921034666</v>
+      </c>
+      <c r="D3">
+        <f>LOG10(0.0333/2.88)</f>
+        <v>-1.9369482542529108</v>
+      </c>
+      <c r="E3">
+        <f>LOG10(0.962/2.88)</f>
+        <v>-0.4762174157214179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1000000</v>
       </c>
       <c r="B4">
-        <f>LOG10(16.132)</f>
-        <v>1.2076882133355811</v>
+        <f>LOG10(14.7)</f>
+        <v>1.167317334748176</v>
       </c>
       <c r="C4">
-        <f>LOG10(0.0631)</f>
-        <v>-1.1999706407558657</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <f>LOG10(0.149/2.87)</f>
+        <v>-1.2846956283217184</v>
+      </c>
+      <c r="D4">
+        <f>LOG10(0.0338/2.87)</f>
+        <v>-1.9289651964563377</v>
+      </c>
+      <c r="E4">
+        <f>LOG10(0.979/2.87)</f>
+        <v>-0.46709920493085455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10000000</v>
       </c>
       <c r="B5">
-        <f>LOG10(26.6)</f>
-        <v>1.424881636631067</v>
+        <f>LOG10(21.4)</f>
+        <v>1.3304137733491908</v>
       </c>
       <c r="C5">
-        <f>LOG10(0.0398)</f>
-        <v>-1.4001169279263121</v>
+        <f>LOG10(0.0904/2.86)</f>
+        <v>-1.5001976026536796</v>
+      </c>
+      <c r="D5">
+        <f>LOG10(0.0488/2.86)</f>
+        <v>-1.7679462111263322</v>
+      </c>
+      <c r="E5">
+        <f>LOG10(1.22/2.86)</f>
+        <v>-0.37000620245429477</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B7">
+        <f>LOG10(17.2)</f>
+        <v>1.2355284469075489</v>
+      </c>
+      <c r="C7">
+        <f>LOG10(0.159/3.07)</f>
+        <v>-1.285741251156735</v>
+      </c>
+      <c r="D7">
+        <f>LOG10((0.0512)/3.07)</f>
+        <v>-1.7778684145013557</v>
+      </c>
+      <c r="E7">
+        <f>LOG10(1.33/3.07)</f>
+        <v>-0.36328673451010068</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B8">
+        <f>LOG10(13.9)</f>
+        <v>1.1430148002540952</v>
+      </c>
+      <c r="C8">
+        <f>LOG10(0.153/3.07)</f>
+        <v>-1.3024469446595877</v>
+      </c>
+      <c r="D8">
+        <f>LOG10((0.045)/3.07)</f>
+        <v>-1.8339258617018428</v>
+      </c>
+      <c r="E8">
+        <f>LOG10(1.22/3.07)</f>
+        <v>-0.40077854480243824</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B9">
+        <f>LOG10(14.2)</f>
+        <v>1.1522883443830565</v>
+      </c>
+      <c r="C9">
+        <f>LOG10(0.18/3.07)</f>
+        <v>-1.2318658703738805</v>
+      </c>
+      <c r="D9">
+        <f>LOG10((0.0484)/3.07)</f>
+        <v>-1.802293013832774</v>
+      </c>
+      <c r="E9">
+        <f>LOG10(1.28/3.07)</f>
+        <v>-0.37992840582931808</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="B10">
+        <f>LOG10(24.3)</f>
+        <v>1.3856062735983121</v>
+      </c>
+      <c r="C10">
+        <f>LOG10(0.109/3.07)</f>
+        <v>-1.4497118775365629</v>
+      </c>
+      <c r="D10">
+        <f>LOG10((0.0798)/3.07)</f>
+        <v>-1.5851354841264571</v>
+      </c>
+      <c r="E10">
+        <f>LOG10(1.76/3.07)</f>
+        <v>-0.24162570766303665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Draft of poster.  I had slacked it to you but I wasn't sure if you had seen it or not.
</commit_message>
<xml_diff>
--- a/Cloudy_Data/LineRatios.xlsx
+++ b/Cloudy_Data/LineRatios.xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -446,20 +446,20 @@
         <v>10000</v>
       </c>
       <c r="B2" s="1">
-        <f>LOG10(15.7)</f>
-        <v>1.1958996524092338</v>
+        <f>LOG10(17.2)</f>
+        <v>1.2355284469075489</v>
       </c>
       <c r="C2">
-        <f>LOG10(0.159/2.86)</f>
-        <v>-1.2549689088085916</v>
+        <f>LOG10(0.355/3.07)</f>
+        <v>-0.93691002242209243</v>
       </c>
       <c r="D2">
-        <f>LOG10(0.0355/2.86)</f>
-        <v>-1.9061376800739489</v>
+        <f>LOG10(0.0355/3.07)</f>
+        <v>-1.9369100224220925</v>
       </c>
       <c r="E2">
-        <f>LOG10(1.01/2.86)</f>
-        <v>-0.45204465934640037</v>
+        <f>LOG10(1.33/3.07)</f>
+        <v>-0.36328673451010068</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -467,20 +467,20 @@
         <v>100000</v>
       </c>
       <c r="B3">
-        <f>LOG10(12.9)</f>
-        <v>1.110589710299249</v>
+        <f>LOG10(13.9)</f>
+        <v>1.1430148002540952</v>
       </c>
       <c r="C3">
-        <f>LOG10(0.131/2.88)</f>
-        <v>-1.3421211921034666</v>
+        <f>LOG10(0.342/3.07)</f>
+        <v>-0.95311226942105143</v>
       </c>
       <c r="D3">
-        <f>LOG10(0.0333/2.88)</f>
-        <v>-1.9369482542529108</v>
+        <f>LOG10(0.045/3.07)</f>
+        <v>-1.8339258617018428</v>
       </c>
       <c r="E3">
-        <f>LOG10(0.962/2.88)</f>
-        <v>-0.4762174157214179</v>
+        <f>LOG10(1.22/3.07)</f>
+        <v>-0.40077854480243824</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -492,16 +492,16 @@
         <v>1.167317334748176</v>
       </c>
       <c r="C4">
-        <f>LOG10(0.149/2.87)</f>
-        <v>-1.2846956283217184</v>
+        <f>LOG10(0.401/3.07)</f>
+        <v>-0.88399400285700414</v>
       </c>
       <c r="D4">
-        <f>LOG10(0.0338/2.87)</f>
-        <v>-1.9289651964563377</v>
+        <f>LOG10(0.0484/3.07)</f>
+        <v>-1.802293013832774</v>
       </c>
       <c r="E4">
-        <f>LOG10(0.979/2.87)</f>
-        <v>-0.46709920493085455</v>
+        <f>LOG10(1.28/3.07)</f>
+        <v>-0.37992840582931808</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -509,20 +509,20 @@
         <v>10000000</v>
       </c>
       <c r="B5">
-        <f>LOG10(21.4)</f>
-        <v>1.3304137733491908</v>
+        <f>LOG10(24.3)</f>
+        <v>1.3856062735983121</v>
       </c>
       <c r="C5">
-        <f>LOG10(0.0904/2.86)</f>
-        <v>-1.5001976026536796</v>
+        <f>LOG10(0.241/3.09)</f>
+        <v>-1.1079414368499663</v>
       </c>
       <c r="D5">
-        <f>LOG10(0.0488/2.86)</f>
-        <v>-1.7679462111263322</v>
+        <f>LOG10(0.0798/3.09)</f>
+        <v>-1.5879555880741052</v>
       </c>
       <c r="E5">
-        <f>LOG10(1.22/2.86)</f>
-        <v>-0.37000620245429477</v>
+        <f>LOG10(1.76/3.09)</f>
+        <v>-0.24444581161068482</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Was able to quickly replot the new values over the groves images.  Apparently I didn't save the right .in file for SEDT6, and I still have the data from SURF in place of it.  It looks a bit better, but we are still much farther off than we'd like.
</commit_message>
<xml_diff>
--- a/Cloudy_Data/LineRatios.xlsx
+++ b/Cloudy_Data/LineRatios.xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -446,20 +446,20 @@
         <v>10000</v>
       </c>
       <c r="B2" s="1">
-        <f>LOG10(17.2)</f>
-        <v>1.2355284469075489</v>
+        <f>LOG10(17.3)</f>
+        <v>1.2380461031287955</v>
       </c>
       <c r="C2">
-        <f>LOG10(0.355/3.07)</f>
-        <v>-0.93691002242209243</v>
+        <f>LOG10(0.329/2.86)</f>
+        <v>-0.93917013517906867</v>
       </c>
       <c r="D2">
-        <f>LOG10(0.0355/3.07)</f>
-        <v>-1.9369100224220925</v>
+        <f>LOG10(0.0476/2.86)</f>
+        <v>-1.7787590804085498</v>
       </c>
       <c r="E2">
-        <f>LOG10(1.33/3.07)</f>
-        <v>-0.36328673451010068</v>
+        <f>LOG10(1.24/2.86)</f>
+        <v>-0.36294434796680791</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -467,20 +467,20 @@
         <v>100000</v>
       </c>
       <c r="B3">
-        <f>LOG10(13.9)</f>
-        <v>1.1430148002540952</v>
+        <f>LOG10(17.3)</f>
+        <v>1.2380461031287955</v>
       </c>
       <c r="C3">
-        <f>LOG10(0.342/3.07)</f>
-        <v>-0.95311226942105143</v>
+        <f>LOG10(0.345/3.06)</f>
+        <v>-0.94790233140830593</v>
       </c>
       <c r="D3">
-        <f>LOG10(0.045/3.07)</f>
-        <v>-1.8339258617018428</v>
+        <f>LOG10(0.0457/3.09)</f>
+        <v>-1.8300422793549844</v>
       </c>
       <c r="E3">
-        <f>LOG10(1.22/3.07)</f>
-        <v>-0.40077854480243824</v>
+        <f>LOG10(1.23/3.09)</f>
+        <v>-0.40005336798543673</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -509,104 +509,40 @@
         <v>10000000</v>
       </c>
       <c r="B5">
-        <f>LOG10(24.3)</f>
-        <v>1.3856062735983121</v>
+        <f>LOG10(24.8)</f>
+        <v>1.3944516808262162</v>
       </c>
       <c r="C5">
-        <f>LOG10(0.241/3.09)</f>
-        <v>-1.1079414368499663</v>
+        <f>LOG10(0.221/2.86)</f>
+        <v>-1.1119737594439323</v>
       </c>
       <c r="D5">
-        <f>LOG10(0.0798/3.09)</f>
-        <v>-1.5879555880741052</v>
+        <f>LOG10(0.0735/2.86)</f>
+        <v>-1.5900786940448481</v>
       </c>
       <c r="E5">
-        <f>LOG10(1.76/3.09)</f>
-        <v>-0.24444581161068482</v>
+        <f>LOG10(1.62/2.86)</f>
+        <v>-0.24685101858641204</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10000</v>
       </c>
-      <c r="B7">
-        <f>LOG10(17.2)</f>
-        <v>1.2355284469075489</v>
-      </c>
-      <c r="C7">
-        <f>LOG10(0.159/3.07)</f>
-        <v>-1.285741251156735</v>
-      </c>
-      <c r="D7">
-        <f>LOG10((0.0512)/3.07)</f>
-        <v>-1.7778684145013557</v>
-      </c>
-      <c r="E7">
-        <f>LOG10(1.33/3.07)</f>
-        <v>-0.36328673451010068</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100000</v>
       </c>
-      <c r="B8">
-        <f>LOG10(13.9)</f>
-        <v>1.1430148002540952</v>
-      </c>
-      <c r="C8">
-        <f>LOG10(0.153/3.07)</f>
-        <v>-1.3024469446595877</v>
-      </c>
-      <c r="D8">
-        <f>LOG10((0.045)/3.07)</f>
-        <v>-1.8339258617018428</v>
-      </c>
-      <c r="E8">
-        <f>LOG10(1.22/3.07)</f>
-        <v>-0.40077854480243824</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1000000</v>
       </c>
-      <c r="B9">
-        <f>LOG10(14.2)</f>
-        <v>1.1522883443830565</v>
-      </c>
-      <c r="C9">
-        <f>LOG10(0.18/3.07)</f>
-        <v>-1.2318658703738805</v>
-      </c>
-      <c r="D9">
-        <f>LOG10((0.0484)/3.07)</f>
-        <v>-1.802293013832774</v>
-      </c>
-      <c r="E9">
-        <f>LOG10(1.28/3.07)</f>
-        <v>-0.37992840582931808</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10000000</v>
-      </c>
-      <c r="B10">
-        <f>LOG10(24.3)</f>
-        <v>1.3856062735983121</v>
-      </c>
-      <c r="C10">
-        <f>LOG10(0.109/3.07)</f>
-        <v>-1.4497118775365629</v>
-      </c>
-      <c r="D10">
-        <f>LOG10((0.0798)/3.07)</f>
-        <v>-1.5851354841264571</v>
-      </c>
-      <c r="E10">
-        <f>LOG10(1.76/3.07)</f>
-        <v>-0.24162570766303665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>